<commit_message>
- Realiza a busca exata por Categorias.
</commit_message>
<xml_diff>
--- a/arquivo.xlsx
+++ b/arquivo.xlsx
@@ -485,6 +485,11 @@
           <t>1/1</t>
         </is>
       </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>TRANSPORTE</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -535,6 +540,11 @@
           <t>1/1</t>
         </is>
       </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>TRANSPORTE</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -860,6 +870,11 @@
           <t>1/1</t>
         </is>
       </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>TRANSPORTE</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -885,6 +900,11 @@
           <t>1/1</t>
         </is>
       </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>ALIMENTAÇÃO</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -1010,6 +1030,11 @@
           <t>1/1</t>
         </is>
       </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>ALIMENTAÇÃO</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -1035,6 +1060,11 @@
           <t>1/1</t>
         </is>
       </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>LAZER</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -1085,6 +1115,11 @@
           <t>1/1</t>
         </is>
       </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>ALIMENTAÇÃO</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -1110,6 +1145,11 @@
           <t>1/1</t>
         </is>
       </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>LAZER</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -1135,6 +1175,11 @@
           <t>1/1</t>
         </is>
       </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>ALIMENTAÇÃO</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -1160,6 +1205,11 @@
           <t>1/1</t>
         </is>
       </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>LAZER</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -1235,6 +1285,11 @@
           <t>1/1</t>
         </is>
       </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>TRANSFERÊNCIA</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
@@ -1285,6 +1340,11 @@
           <t>1/1</t>
         </is>
       </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>TRANSPORTE</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
@@ -1310,6 +1370,11 @@
           <t>1/1</t>
         </is>
       </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>TRANSPORTE</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
@@ -1360,6 +1425,11 @@
           <t>1/1</t>
         </is>
       </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>TRANSPORTE</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
@@ -1385,6 +1455,11 @@
           <t>1/1</t>
         </is>
       </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>TRANSPORTE</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
@@ -1510,6 +1585,11 @@
           <t>1/1</t>
         </is>
       </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>TRANSPORTE</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
@@ -1535,6 +1615,11 @@
           <t>1/1</t>
         </is>
       </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>TRANSPORTE</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
@@ -1560,6 +1645,11 @@
           <t>1/1</t>
         </is>
       </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>STREAMING</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
@@ -1585,6 +1675,11 @@
           <t>1/1</t>
         </is>
       </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>TRANSPORTE</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
@@ -1635,6 +1730,11 @@
           <t>1/1</t>
         </is>
       </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>TRANSPORTE</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
@@ -1660,6 +1760,11 @@
           <t>1/1</t>
         </is>
       </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>TRANSPORTE</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
@@ -1760,6 +1865,11 @@
           <t>1/1</t>
         </is>
       </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>LAZER</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
@@ -1785,6 +1895,11 @@
           <t>1/1</t>
         </is>
       </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>LAZER</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
@@ -1985,6 +2100,11 @@
           <t>1/1</t>
         </is>
       </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>ALIMENTAÇÃO</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
@@ -2260,6 +2380,11 @@
           <t>1/1</t>
         </is>
       </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>LAZER</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
@@ -2285,6 +2410,11 @@
           <t>1/1</t>
         </is>
       </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>TRANSPORTE</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
@@ -2410,6 +2540,11 @@
           <t>1/1</t>
         </is>
       </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>MERCADO</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
@@ -2485,6 +2620,11 @@
           <t>1/1</t>
         </is>
       </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>MERCADO</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
@@ -2510,6 +2650,11 @@
           <t>1/1</t>
         </is>
       </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>MERCADO</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
@@ -2535,6 +2680,11 @@
           <t>1/1</t>
         </is>
       </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>OUTROS</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
@@ -2560,6 +2710,11 @@
           <t>1/2</t>
         </is>
       </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>OUTROS</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
@@ -2585,6 +2740,11 @@
           <t>1/1</t>
         </is>
       </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>STREAMING</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
@@ -2760,6 +2920,11 @@
           <t>1/1</t>
         </is>
       </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>LAZER</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
@@ -2785,6 +2950,11 @@
           <t>1/1</t>
         </is>
       </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>SAÚDE</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
@@ -2810,6 +2980,11 @@
           <t>1/1</t>
         </is>
       </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>TRANSPORTE</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
@@ -2835,6 +3010,11 @@
           <t>1/1</t>
         </is>
       </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>TRANSPORTE</t>
+        </is>
+      </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
@@ -2860,6 +3040,11 @@
           <t>1/1</t>
         </is>
       </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>LAZER</t>
+        </is>
+      </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="n">
@@ -2935,6 +3120,11 @@
           <t>1/1</t>
         </is>
       </c>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>LAZER</t>
+        </is>
+      </c>
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
@@ -2960,6 +3150,11 @@
           <t>1/2</t>
         </is>
       </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>OUTROS</t>
+        </is>
+      </c>
     </row>
     <row r="102">
       <c r="A102" s="1" t="n">
@@ -2985,6 +3180,11 @@
           <t>1/1</t>
         </is>
       </c>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>ALIMENTAÇÃO</t>
+        </is>
+      </c>
     </row>
     <row r="103">
       <c r="A103" s="1" t="n">
@@ -3010,6 +3210,11 @@
           <t>1/1</t>
         </is>
       </c>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>TRANSPORTE</t>
+        </is>
+      </c>
     </row>
     <row r="104">
       <c r="A104" s="1" t="n">
@@ -3035,6 +3240,11 @@
           <t>1/1</t>
         </is>
       </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>TRANSPORTE</t>
+        </is>
+      </c>
     </row>
     <row r="105">
       <c r="A105" s="1" t="n">
@@ -3085,6 +3295,11 @@
           <t>1/1</t>
         </is>
       </c>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>LAZER</t>
+        </is>
+      </c>
     </row>
     <row r="107">
       <c r="A107" s="1" t="n">
@@ -3110,6 +3325,11 @@
           <t>1/1</t>
         </is>
       </c>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>LAZER</t>
+        </is>
+      </c>
     </row>
     <row r="108">
       <c r="A108" s="1" t="n">
@@ -3135,6 +3355,11 @@
           <t>1/2</t>
         </is>
       </c>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>OUTROS</t>
+        </is>
+      </c>
     </row>
     <row r="109">
       <c r="A109" s="1" t="n">
@@ -3160,6 +3385,11 @@
           <t>1/1</t>
         </is>
       </c>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t>TRANSPORTE</t>
+        </is>
+      </c>
     </row>
     <row r="110">
       <c r="A110" s="1" t="n">
@@ -3185,6 +3415,11 @@
           <t>1/1</t>
         </is>
       </c>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t>TRANSPORTE</t>
+        </is>
+      </c>
     </row>
     <row r="111">
       <c r="A111" s="1" t="n">
@@ -3260,6 +3495,11 @@
           <t>1/1</t>
         </is>
       </c>
+      <c r="F113" t="inlineStr">
+        <is>
+          <t>TRANSPORTE</t>
+        </is>
+      </c>
     </row>
     <row r="114">
       <c r="A114" s="1" t="n">
@@ -3360,6 +3600,11 @@
           <t>1/1</t>
         </is>
       </c>
+      <c r="F117" t="inlineStr">
+        <is>
+          <t>TRANSPORTE</t>
+        </is>
+      </c>
     </row>
     <row r="118">
       <c r="A118" s="1" t="n">
@@ -3385,6 +3630,11 @@
           <t>1/1</t>
         </is>
       </c>
+      <c r="F118" t="inlineStr">
+        <is>
+          <t>TRANSPORTE</t>
+        </is>
+      </c>
     </row>
     <row r="119">
       <c r="A119" s="1" t="n">
@@ -3435,6 +3685,11 @@
           <t>1/1</t>
         </is>
       </c>
+      <c r="F120" t="inlineStr">
+        <is>
+          <t>TRANSPORTE</t>
+        </is>
+      </c>
     </row>
     <row r="121">
       <c r="A121" s="1" t="n">
@@ -3485,6 +3740,11 @@
           <t>1/1</t>
         </is>
       </c>
+      <c r="F122" t="inlineStr">
+        <is>
+          <t>TRANSPORTE</t>
+        </is>
+      </c>
     </row>
     <row r="123">
       <c r="A123" s="1" t="n">
@@ -3535,6 +3795,11 @@
           <t>1/1</t>
         </is>
       </c>
+      <c r="F124" t="inlineStr">
+        <is>
+          <t>TRANSPORTE</t>
+        </is>
+      </c>
     </row>
     <row r="125">
       <c r="A125" s="1" t="n">
@@ -3558,6 +3823,11 @@
       <c r="E125" t="inlineStr">
         <is>
           <t>1/1</t>
+        </is>
+      </c>
+      <c r="F125" t="inlineStr">
+        <is>
+          <t>TRANSPORTE</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
- Implementa a busca por similaridade.
</commit_message>
<xml_diff>
--- a/arquivo.xlsx
+++ b/arquivo.xlsx
@@ -745,6 +745,11 @@
           <t>1/1</t>
         </is>
       </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>ALIMENTAÇÃO</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -980,6 +985,11 @@
           <t>1/1</t>
         </is>
       </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>ALIMENTAÇÃO</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -1005,6 +1015,11 @@
           <t>1/1</t>
         </is>
       </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>ALIMENTAÇÃO</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -2440,6 +2455,11 @@
           <t>1/1</t>
         </is>
       </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>ALIMENTAÇÃO</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
@@ -2820,6 +2840,11 @@
           <t>1/1</t>
         </is>
       </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>COMPRAS</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
@@ -2895,6 +2920,11 @@
           <t>1/1</t>
         </is>
       </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>ALIMENTAÇÃO</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
@@ -3095,6 +3125,11 @@
           <t>1/1</t>
         </is>
       </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>LAZER</t>
+        </is>
+      </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
@@ -3660,6 +3695,11 @@
           <t>1/1</t>
         </is>
       </c>
+      <c r="F119" t="inlineStr">
+        <is>
+          <t>TRANSPORTE</t>
+        </is>
+      </c>
     </row>
     <row r="120">
       <c r="A120" s="1" t="n">
@@ -3770,6 +3810,11 @@
           <t>1/1</t>
         </is>
       </c>
+      <c r="F123" t="inlineStr">
+        <is>
+          <t>TRANSPORTE</t>
+        </is>
+      </c>
     </row>
     <row r="124">
       <c r="A124" s="1" t="n">
@@ -3855,6 +3900,11 @@
           <t>1/1</t>
         </is>
       </c>
+      <c r="F126" t="inlineStr">
+        <is>
+          <t>MERCADO</t>
+        </is>
+      </c>
     </row>
     <row r="127">
       <c r="A127" s="1" t="n">
@@ -3930,6 +3980,11 @@
           <t>1/1</t>
         </is>
       </c>
+      <c r="F129" t="inlineStr">
+        <is>
+          <t>CARRO</t>
+        </is>
+      </c>
     </row>
     <row r="130">
       <c r="A130" s="1" t="n">
@@ -3953,6 +4008,11 @@
       <c r="E130" t="inlineStr">
         <is>
           <t>1/1</t>
+        </is>
+      </c>
+      <c r="F130" t="inlineStr">
+        <is>
+          <t>ALIMENTAÇÃO</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
- Implementa Feature Toggle e conclui busca_ai.
</commit_message>
<xml_diff>
--- a/arquivo.xlsx
+++ b/arquivo.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,16 +463,16 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>45231</v>
+        <v>45235</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Sancto Churrasco</t>
+          <t>Point Da Irae</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>-201,08</t>
+          <t>-60,00</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -488,21 +488,21 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>45231</v>
+        <v>45235</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Aga</t>
+          <t>Boteco Parô</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>-8,00</t>
+          <t>-343,39</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>CINTHIA</t>
+          <t>PHILIPPE</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -513,21 +513,21 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>45231</v>
+        <v>45235</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Abastece Ai</t>
+          <t>Cuor Di Crema</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>-225,40</t>
+          <t>-19,50</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>PHILIPPE</t>
+          <t>CINTHIA</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -538,16 +538,16 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>45231</v>
+        <v>45235</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Enel</t>
+          <t>Emporium Sao Paulo</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>-225,71</t>
+          <t>-15,00</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -563,96 +563,101 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>45231</v>
+        <v>45234</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Mercado Livre</t>
+          <t>Uber</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>-67,36</t>
+          <t>-29,97</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>CINTHIA</t>
+          <t>PHILIPPE</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
           <t>1/1</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>TRANSPORTE</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>45231</v>
+        <v>45234</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Mercado Livre</t>
+          <t>Top</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>-183,04</t>
+          <t>-8,80</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>CINTHIA</t>
+          <t>PHILIPPE</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
           <t>1/1</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>TRANSPORTE</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>45230</v>
+        <v>45234</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Uber</t>
+          <t>Motorsport</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>-25,46</t>
+          <t>-300,00</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>CINTHIA</t>
+          <t>PHILIPPE</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
           <t>1/1</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>TRANSPORTE</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>45230</v>
+        <v>45234</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Uber</t>
+          <t>Caldo De Cana Da</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>-28,92</t>
+          <t>-8,00</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -663,26 +668,21 @@
       <c r="E9" t="inlineStr">
         <is>
           <t>1/1</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>TRANSPORTE</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>45229</v>
+        <v>45234</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Nestlé</t>
+          <t>Alem Do Hamburguer</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>-91,80</t>
+          <t>-20,00</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -693,31 +693,26 @@
       <c r="E10" t="inlineStr">
         <is>
           <t>1/1</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>MERCADO</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>45229</v>
+        <v>45234</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Uber</t>
+          <t>Top</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>-16,95</t>
+          <t>-17,60</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>CINTHIA</t>
+          <t>PHILIPPE</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -733,21 +728,21 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>45229</v>
+        <v>45233</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Moema Service</t>
+          <t>Saru Sushi</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>-30,00</t>
+          <t>-650,87</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>PHILIPPE</t>
+          <t>CINTHIA</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -758,31 +753,516 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>45229</v>
+        <v>45233</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Uber</t>
+          <t>Bar Jobim</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>-56,49</t>
+          <t>-48,18</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
+          <t>PHILIPPE</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>LAZER</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>45233</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Bar Jobim</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>-100,00</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>PHILIPPE</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>LAZER</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>45233</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Centauro</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>-179,99</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
           <t>CINTHIA</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>1/1</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>TRANSPORTE</t>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>1/2</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>45233</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Panvel</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>-183,80</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>CINTHIA</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>1/2</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>45233</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Panvel</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>-0,00</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>CINTHIA</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>45233</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Oba Hortifruti</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>-82,04</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>PHILIPPE</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>MERCADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>45233</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Swift</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>-55,96</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>PHILIPPE</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>MERCADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>45233</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Senhora Adega</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>-45,99</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>PHILIPPE</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>45233</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Echope</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>-179,64</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>PHILIPPE</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>LAZER</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>45232</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Bar Jobim</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>-90,00</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>CINTHIA</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>LAZER</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>45232</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Bar Jobim</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>-355,57</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>PHILIPPE</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>LAZER</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>45232</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Koa Moema</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>-49,80</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>CINTHIA</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>ALIMENTAÇÃO</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>45232</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Veneza Enxovais Textil</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>-305,52</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>CINTHIA</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>1/2</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>45231</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Sancto Churrasco</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>-201,08</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>PHILIPPE</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>45231</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Aga</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>-8,00</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>CINTHIA</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>45231</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Abastece Ai</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>-225,40</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>PHILIPPE</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>45231</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Enel</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>-225,71</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>PHILIPPE</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>45231</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Mercado Livre</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>-67,36</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>CINTHIA</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>45231</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Mercado Livre</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>-183,04</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>CINTHIA</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>1/1</t>
         </is>
       </c>
     </row>

</xml_diff>